<commit_message>
[daily] Upgrade purchase analyze
</commit_message>
<xml_diff>
--- a/support_data/purchase_analysis/purchase_analysis.xlsx
+++ b/support_data/purchase_analysis/purchase_analysis.xlsx
@@ -19,7 +19,7 @@
     <t>Номенклатура</t>
   </si>
   <si>
-    <t>Дефицит</t>
+    <t>План_закупа</t>
   </si>
   <si>
     <t>Заказано</t>
@@ -28,96 +28,45 @@
     <t>Доставлено</t>
   </si>
   <si>
-    <t>Еще_заказать</t>
-  </si>
-  <si>
-    <t>Болт М12-6gх50.8.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
-    <t>Болт М14-6gх45.8.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
-    <t>Болт М14-6gх45.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
-    <t>Болт М14-6gх50.8.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
-    <t>Болт М14-6gх50.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
-    <t>Болт М14-6gх55.8.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
-    <t>Болт М14-6gх55.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
+    <t>Остаточная_потребность</t>
+  </si>
+  <si>
+    <t>Болт М12-6gх160.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
     <t>Болт М16-6gх50.8.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
-    <t>Болт М16-6gх50.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
-    <t>Болт М16-6gх55.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
+    <t>Болт М16-6gх50.8.8.ТД4 ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
     <t>Болт М18-6gх95.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
-    <t>Болт М20-6gх200.5.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
     <t>Болт М20-6gх200.5.8.Гл ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
-    <t>Болт М20-6gх200.5.8.ТД4 ГОСТ Р ИСО 4014-2013</t>
+    <t>Болт М20-6gх200.8.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
     <t>Болт М20-6gх200.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
-    <t>Болт М20-6gх240.8.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
     <t>Болт М20-6gх240.8.8.бп ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
-    <t>Болт М20-6gх60.8.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
-    <t>Болт М20-6gх60.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
     <t>Болт М20-6gх65.8.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
-    <t>Болт М20-6gх65.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
     <t>Болт М20-6gх65.8.8.ТД4 ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
     <t>Болт М20-6gх65.8.8.бп ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
-    <t>Болт М20-6gх70.8.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
-    <t>Болт М20-6gх70.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
-    <t>Болт М20-6gх90.8.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
-    <t>Болт М20-6gх90.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
     <t>Болт М24-6gх110.8.8.ТД4 ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
-    <t>Болт М24-6gх75.8.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
     <t>Болт М24-6gх75.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
@@ -136,19 +85,10 @@
     <t>Болт М24-6gх85.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
-    <t>Болт М24-6gх90.8.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
     <t>Болт М24-6gх90.8.8.Гл ГОСТ Р 50793-95</t>
   </si>
   <si>
-    <t>Болт М27-6gх80.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
-    <t>Болт М30-6gх115.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
-    <t>Болт М30-6gх90.8.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
+    <t>Болт М27-6gх70.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
     <t>Болт М30-6gх90.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
@@ -163,7 +103,7 @@
     <t>Болт М36-6gх120.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
-    <t>Болт М36-6gх150.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
+    <t>Болт М36-6gх140.8.8.ТД4 ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
     <t>Болт М36-6gх150.8.8.ТД4 ГОСТ Р ИСО 4014-2013</t>
@@ -172,28 +112,22 @@
     <t>Болт М36-6gх150.8.8.бп ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
-    <t>Болт М36-6gх160.5.8.Гл ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
     <t>Болт М36-6gх160.8.8.ГЦ ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
-    <t>Болт М36-6gх160.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
+    <t>Болт М36-6gх160.8.8.ТД4 ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
     <t>Болт М36-6gх160.8.8.бп ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
-    <t>Болт М6-6gх16.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
-  </si>
-  <si>
-    <t>Болт М6-6gх25.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
+    <t>Болт М6-6gх20.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
     <t>Болт М8-6gх100.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
-    <t>Болт М8-6gх25.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
+    <t>Болт М8-6gх35.8.8.Гл ГОСТ 7798-70</t>
   </si>
   <si>
     <t>Болт М8-6gх35.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
@@ -205,30 +139,39 @@
     <t>Болт по чертежу Спецболт М46 М24х525.09Г2С-15.ГЦ Чертёж 3.407.1-175</t>
   </si>
   <si>
+    <t>Болт по чертежу Спецболт М46 М24х525.09Г2С-15.ТД Чертёж 3.407.1-175</t>
+  </si>
+  <si>
     <t>Болт по чертежу Спецболт М47 М24х550.09Г2С-15.ГЦ Чертёж 3.407.1-175</t>
   </si>
   <si>
+    <t>Болт по чертежу Спецболт М47 М24х550.09Г2С-15.ТД Чертёж 3.407.1-175</t>
+  </si>
+  <si>
     <t>Болт по чертежу Спецболт М48 М24х575.09Г2С-15.ГЦ Чертёж 3.407.1-175</t>
   </si>
   <si>
-    <t>Болт самоанкерующийся распорный БСР 16х150 УХЛ3 ГОСТ 28778-90</t>
+    <t>Болт по чертежу Спецболт М48 М24х575.09Г2С-15.ТД Чертёж 3.407.1-175</t>
+  </si>
+  <si>
+    <t>Винт М6-6gх16.8.8.Гл ГОСТ Р ИСО 4014-2013</t>
   </si>
   <si>
     <t>Вязка спиральная ВС-120/150-2</t>
   </si>
   <si>
+    <t>Вязка спиральная ВС-70/95.1</t>
+  </si>
+  <si>
+    <t>Вязка спиральная ПВС70/95-10</t>
+  </si>
+  <si>
     <t>Гайка М10-6h.5.Гл ГОСТ ISO 4032-2014</t>
   </si>
   <si>
-    <t>Гайка М16-6h.5.Гл ГОСТ ISO 4032-2014</t>
-  </si>
-  <si>
     <t>Гайка М16-6h.8.ГЦ ГОСТ ISO 4032-2014</t>
   </si>
   <si>
-    <t>Гайка М16-6h.8.Гл ГОСТ ISO 4032-2014</t>
-  </si>
-  <si>
     <t>Гайка М16-6h.8.ТД4 ГОСТ ISO 4032-2014</t>
   </si>
   <si>
@@ -262,15 +205,9 @@
     <t>Гайка М30-6h.8.ГЦ ГОСТ ISO 4032-2014</t>
   </si>
   <si>
-    <t>Гайка М30-6h.8.Гл ГОСТ ISO 4032-2014</t>
-  </si>
-  <si>
     <t>Гайка М30-6h.8.ТД4 ГОСТ ISO 4032-2014</t>
   </si>
   <si>
-    <t>Гайка М36-6h.5.Гл ГОСТ ISO 4032-2014</t>
-  </si>
-  <si>
     <t>Гайка М36-6h.8.ГЦ ГОСТ ISO 4032-2014</t>
   </si>
   <si>
@@ -286,10 +223,19 @@
     <t>Гайка М42-6h.8.бп ГОСТ ISO 4032-2014</t>
   </si>
   <si>
-    <t>Зажим клыковый КС-185-1</t>
-  </si>
-  <si>
-    <t>Зажим натяжной Н3-2-7</t>
+    <t>Гайка М48-6h.8.ГЦ ГОСТ ISO 4032-2014</t>
+  </si>
+  <si>
+    <t>Зажим ЗПС-120-3В</t>
+  </si>
+  <si>
+    <t>Зажим ПА-1-1</t>
+  </si>
+  <si>
+    <t>Зажим ПАМ-3-1 ТУ 3449-021-59116459-06</t>
+  </si>
+  <si>
+    <t>Зажим аппаратный А2А-120-Т</t>
   </si>
   <si>
     <t>Зажим натяжной НБ-2-6</t>
@@ -298,31 +244,40 @@
     <t>Зажим натяжной НБ-3-6Б</t>
   </si>
   <si>
-    <t>Зажим натяжной НБ-60/5,6-16</t>
-  </si>
-  <si>
-    <t>Зажим поддерживающий ПГ-30/12-20</t>
-  </si>
-  <si>
-    <t>Зажим поддерживающий ПГН-5-3</t>
-  </si>
-  <si>
-    <t>Зажим прокалывающий ОАЗ-1с кожухом К3-02</t>
-  </si>
-  <si>
-    <t>Заклепка 4х14 DIN 7337</t>
-  </si>
-  <si>
-    <t>Звено (талреп) ПТР-12-1</t>
-  </si>
-  <si>
-    <t>Изолятор ЛК 70/10 -4СП</t>
-  </si>
-  <si>
-    <t>Изолятор ЛК 70/35-4 СП</t>
-  </si>
-  <si>
-    <t>Изолятор ЛК120/10-4 СП</t>
+    <t>Зажим плашечный ПА-2-2</t>
+  </si>
+  <si>
+    <t>Зажим поддерживающий ПГН-2-6</t>
+  </si>
+  <si>
+    <t>Зажим поддерживающий ПГН-3-5</t>
+  </si>
+  <si>
+    <t>Звено ПР-7-6</t>
+  </si>
+  <si>
+    <t>Звено ПРВ-12-1 ТУ 3449-109-00111120-95</t>
+  </si>
+  <si>
+    <t>Звено ПРР-12-1А ТУ 3449-109-00111120-95</t>
+  </si>
+  <si>
+    <t>Звено ПРР-7-1 ТУ 3449-109-00111120-95</t>
+  </si>
+  <si>
+    <t>Звено ПРТ-7-1 ТУ 3449-109-00111120-95</t>
+  </si>
+  <si>
+    <t>Звено ПТМ-12-2 ТУ 3449-109-00111120-95</t>
+  </si>
+  <si>
+    <t>Звено ПТМ-12-3А ТУ 34 49-109-00111120-95</t>
+  </si>
+  <si>
+    <t>Звено ПТМ-7-2 ТУ 3449-109-00111120-95</t>
+  </si>
+  <si>
+    <t>Звено ПТМ-7-3A ТУ 34 49-109-00111120-95</t>
   </si>
   <si>
     <t>Изолятор ЛК120/35-4 СП</t>
@@ -331,25 +286,70 @@
     <t>Изолятор ЛК70/10-4СП</t>
   </si>
   <si>
-    <t>Изолятор ЛОК 12,5-10-4-20-50 УХЛ1 исп.1</t>
-  </si>
-  <si>
-    <t>Изолятор ЛОК 12,5-20-4-20-50 УХЛ1 исп.1</t>
-  </si>
-  <si>
-    <t>Изолятор ЛОК 12,5-35-4-20-50 УХЛ1 исп.1</t>
-  </si>
-  <si>
-    <t>Изолятор ШП 10-4 УХЛ1</t>
+    <t>Кабель силовой ВВГнг(А)-LS 5х2,5</t>
+  </si>
+  <si>
+    <t>Кабель силовой бронированный ВБШвнг(А)-ХЛ 5х2,5-1</t>
+  </si>
+  <si>
+    <t>Канат 15-Г-Ж-1770/ГОСТ 3066-80</t>
+  </si>
+  <si>
+    <t>Карабин DIN 5299С 7х70</t>
   </si>
   <si>
     <t>Колпачок К-6</t>
   </si>
   <si>
-    <t>Коромысло К2-12-2</t>
-  </si>
-  <si>
-    <t>Коуш 45ХЛ ГОСТ 2224-93</t>
+    <t>Коробка клеммная с наборными зажимами КЗНС-32, IP65, УХЛ1,5</t>
+  </si>
+  <si>
+    <t>Коробка клеммная, 3 ввода для металлорукава Dy25 (кабель 8-16мм), IP54, УХЛ1</t>
+  </si>
+  <si>
+    <t>Коробка клеммная, 5 вводов для металлорукава Dy25 (кабель 8-16мм), IP54, УХЛ1</t>
+  </si>
+  <si>
+    <t>Коробка клеммная, 6 вводов для металлорукава Dy25 (кабель 8-16мм), IP54, УХЛ1</t>
+  </si>
+  <si>
+    <t>Кронштейн ВОЛС "УК(У)-125"</t>
+  </si>
+  <si>
+    <t>Лента монтажная стальная в кассете F2007  E</t>
+  </si>
+  <si>
+    <t>Петля М14 ОЭМЗ.ПБ.261.04.02.001</t>
+  </si>
+  <si>
+    <t>Пробойник_СП-13</t>
+  </si>
+  <si>
+    <t>Пробойник_СП-17</t>
+  </si>
+  <si>
+    <t>Пробойник_СП-21</t>
+  </si>
+  <si>
+    <t>Пробойник_СП-25</t>
+  </si>
+  <si>
+    <t>Пробойник_СП-28</t>
+  </si>
+  <si>
+    <t>Пробойник_СП-31</t>
+  </si>
+  <si>
+    <t>Провод заземляющий ПуГВ-ХЛ 1х6мм2</t>
+  </si>
+  <si>
+    <t>Прожектор "Факел Р-2х400Ж" ЖКУ 26-2х400-005 U=220В,IР65,УХЛ1 в комп с 2 лампами ДНаТ-400,2мя ПРА</t>
+  </si>
+  <si>
+    <t>Птицезащитное устройство ПЗУ -S</t>
+  </si>
+  <si>
+    <t>Птицезащитное устройство ПЗУ -SА</t>
   </si>
   <si>
     <t>Птицезащитное устройство ПЗУ-6-10 кВ-ds</t>
@@ -358,46 +358,52 @@
     <t>Птицезащитное устройство ПЗУ-6-10 кВ-line</t>
   </si>
   <si>
-    <t>Птицезащитное устройство ПЗУ-6-35 кВ-GP-d46</t>
-  </si>
-  <si>
     <t>Птицезащитное устройство ПЗУ-GP</t>
   </si>
   <si>
-    <t>Разрядник РМК-20-IV-УХЛ1/021</t>
-  </si>
-  <si>
-    <t>Разрядник РМК-С-20-IV-УХЛ1/021</t>
-  </si>
-  <si>
-    <t>Разрядник РМКЭ-35-IV-УХЛ1</t>
+    <t>Разбавитель 648</t>
+  </si>
+  <si>
+    <t>Разбавитель Сольвент</t>
   </si>
   <si>
     <t>Саморез KPcZP 5,5х38 №5 (удлинн. сверло) Tech  KREP</t>
   </si>
   <si>
+    <t>Светодиодный светильник FНВ 34-600-850-С120,IP66,УХЛ1</t>
+  </si>
+  <si>
+    <t>Серьга СР-12-16 ТУ 3449-105-00111120-94</t>
+  </si>
+  <si>
+    <t>Серьга СР-7-16 ГОСТ 2725-78</t>
+  </si>
+  <si>
     <t>Скоба СК-12-1А</t>
   </si>
   <si>
     <t>Скоба СК-7-1А</t>
   </si>
   <si>
-    <t>Скоба СКД -10-1.</t>
-  </si>
-  <si>
     <t>Скоба СКД-12-1</t>
   </si>
   <si>
-    <t>Скоба СКТ-12-1</t>
-  </si>
-  <si>
-    <t>Спиральная вязка ВС 70/95.2</t>
+    <t>Скоба однолапковая СМО 16-17мм под болт М6</t>
+  </si>
+  <si>
+    <t>Табличка 63х80 12Х18Н10Т</t>
+  </si>
+  <si>
+    <t>Узел крепления КГ-12-1 ТУ 3449-108-00111120-94</t>
   </si>
   <si>
     <t>Узел крепления КГП-7-1</t>
   </si>
   <si>
-    <t>Устройство защиты от перенапряжений УЗПН-6-ЛК УХЛ1</t>
+    <t>Узел крепления КГП-7-2Б ТУ 3449-108-00111120-94</t>
+  </si>
+  <si>
+    <t>Ушко У-1-7-16</t>
   </si>
   <si>
     <t>Ушко У-1-7-16.</t>
@@ -406,28 +412,31 @@
     <t>Ушко У1-12-16 ТУ 3449-111-00111120-95</t>
   </si>
   <si>
+    <t>Ушко У1К-7-16 ТУ 3449-111-00111120-95</t>
+  </si>
+  <si>
+    <t>Ушко У2-7-16 ТУ 3449-111-00111120-95</t>
+  </si>
+  <si>
+    <t>Хомут 728</t>
+  </si>
+  <si>
+    <t>Хомут 730</t>
+  </si>
+  <si>
     <t>Хомут по чертежу 220 20.09Г2С-15.Гл ОЭМЗ.АУ.121.00.00.002</t>
   </si>
   <si>
-    <t>Хомут по чертежу Х-1 20.09Г2С-15.ГЦ Чертёж: ДК10-Х-1.01</t>
-  </si>
-  <si>
     <t>Хомут по чертежу Х-1 20.09Г2С-15.Гл Чертёж: ДК10-Х-1.01</t>
   </si>
   <si>
     <t>Хомут по чертежу Х-1 М20.09Г2С-15.ТД4 Чертёж: ДК10-Х-1.01</t>
   </si>
   <si>
-    <t>Хомут по чертежу Х90-1 12.09Г2С-15.ГЦ ГОСТ К-ТП.10-110-00.07</t>
-  </si>
-  <si>
-    <t>Хомут по чертежу Х90-1 12.09Г2С-15.Гл ГОСТ К-ТП.10-110-00.07</t>
-  </si>
-  <si>
-    <t>Шайба 16 ГЦ ГОСТ 11371-78</t>
-  </si>
-  <si>
-    <t>Шайба 16 ГЦ ГОСТ 6402-70</t>
+    <t>Хомут по чертежу Х2 16.09Г2С-12.Гл 3.407.1-143.8.49</t>
+  </si>
+  <si>
+    <t>Цепь  7,1-1-Т(8)-25 ГОСТ 30441-97</t>
   </si>
   <si>
     <t>Шайба 16 Гл ГОСТ 11371-78</t>
@@ -445,9 +454,6 @@
     <t>Шайба 20 ГЦ ГОСТ 6402-70</t>
   </si>
   <si>
-    <t>Шайба 20 Гл ГОСТ 6402-70</t>
-  </si>
-  <si>
     <t>Шайба 20 ТД4 ГОСТ 6402-70</t>
   </si>
   <si>
@@ -460,13 +466,10 @@
     <t>Шайба 24 ГЦ ГОСТ 6402-70</t>
   </si>
   <si>
-    <t>Шайба 24 Гл ГОСТ 11371-78</t>
-  </si>
-  <si>
     <t>Шайба 24 Гл ГОСТ 6402-70</t>
   </si>
   <si>
-    <t>Шайба 24 ТД4 ГОСТ 11371-78</t>
+    <t>Шайба 24 ТД4 ГОСТ 6402-70</t>
   </si>
   <si>
     <t>Шайба 24 бп ГОСТ 11371-78</t>
@@ -481,18 +484,6 @@
     <t>Шайба 36 бп ГОСТ 11371-78</t>
   </si>
   <si>
-    <t>Шайба 6 Гл ГОСТ 6958-78</t>
-  </si>
-  <si>
-    <t>Шайба A.12 Гл ГОСТ 11371-78</t>
-  </si>
-  <si>
-    <t>Шайба М 36Гл ГОСТ 24379.1-2012</t>
-  </si>
-  <si>
-    <t>Шпилька С3М36-8gх600..Гл ГОСТ 24379.1-2012</t>
-  </si>
-  <si>
     <t>Шпилька по чертежу 12х.09Г2С-8.ТД TER_RecDet_Stud_20</t>
   </si>
   <si>
@@ -508,31 +499,40 @@
     <t>Шпилька по чертежу М36х480.09Г2С-15.ГЦ ОЭМЗ.РМ.252.00.00.001</t>
   </si>
   <si>
+    <t>Шпилька по чертежу М36х480.09Г2С-15.ТД ОЭМЗ.РМ.252.00.00.001</t>
+  </si>
+  <si>
+    <t>Шпилька по чертежу М42х565.09Г2С-15.бп 3.407.9-146.2-000101</t>
+  </si>
+  <si>
     <t>Шпилька по чертежу М42х600.40Х.Гл ОЭМЗ.БМ.076.00.00.001</t>
   </si>
   <si>
-    <t>Шпилька по чертежу Ш-1 М24х350.40Х.ГЦ ДК10-Ш-1.02</t>
-  </si>
-  <si>
     <t>Шпилька по чертежу Ш-1 М24х350.40Х.ТД4 ДК10-Ш-1.02</t>
   </si>
   <si>
     <t>Шпилька по чертежу Ш2 М20х350.40Х.Гл К-ТП.10-110-00.19</t>
   </si>
   <si>
-    <t>Шпилька по чертежу Шп1 М12х440.Ст45.Гл Шп1-00.001</t>
-  </si>
-  <si>
     <t>Шпилька по чертежу Шпк-02 24х.40Х.Гл ОЭМЗ.АУ.121.00.00.001</t>
   </si>
   <si>
     <t>Шпилька по чертежу ф412 48х645.09Г2С-12.бп ОГ-ТП.10/220-ф412</t>
   </si>
   <si>
-    <t>Шплинт 3,2х25.Гл ГОСТ 397-79</t>
+    <t>Шпилька(резьба 115 мм) 7М30-8gх430..бп ГОСТ 24379.1-2012</t>
   </si>
   <si>
     <t>Штырь Ш-20-2-55 ГОСТ 18381-80</t>
+  </si>
+  <si>
+    <t>Эмаль ХВ-110, желтая</t>
+  </si>
+  <si>
+    <t>Эмаль ХВ-110, зеленая</t>
+  </si>
+  <si>
+    <t>Ящик силовой с автомат. выключат., УХЛ1</t>
   </si>
 </sst>
 </file>
@@ -918,7 +918,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0.24081633</v>
+        <v>5.42653061</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -927,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>5.42653061</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -935,7 +935,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>16.34708164</v>
+        <v>107.42685716</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -944,7 +944,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>107.42685716</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -952,16 +952,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>843.9877551299998</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>1080</v>
+        <v>25</v>
       </c>
       <c r="D4">
-        <v>972</v>
+        <v>25</v>
       </c>
       <c r="E4">
-        <v>-236.0122448700002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -969,7 +969,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>29.507</v>
+        <v>8.41020408</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -978,7 +978,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>8.41020408</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -986,16 +986,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>378.1062653299997</v>
+        <v>1508.000965979998</v>
       </c>
       <c r="C6">
-        <v>1080</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>972</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>-701.8937346700003</v>
+        <v>1508.000965979998</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1003,7 +1003,7 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>12.874</v>
+        <v>32.3831102</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1012,7 +1012,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>32.3831102</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1020,7 +1020,7 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>368.5734897900001</v>
+        <v>4050.40766013</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1029,7 +1029,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>4050.40766013</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1037,7 +1037,7 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>252.34138778</v>
+        <v>5.43975284</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1046,7 +1046,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>5.43975284</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1054,16 +1054,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1302.26435427</v>
       </c>
       <c r="C10">
-        <v>1080</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>972</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>-1080</v>
+        <v>1302.26435427</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1071,16 +1071,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>507.945552949999</v>
       </c>
       <c r="C11">
-        <v>1080</v>
+        <v>850</v>
       </c>
       <c r="D11">
-        <v>972</v>
+        <v>850</v>
       </c>
       <c r="E11">
-        <v>-1080</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1088,7 +1088,7 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>8.41020408</v>
+        <v>1.88259526</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1097,7 +1097,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1.88259526</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1105,13 +1105,13 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>4009.30741811</v>
+        <v>16.76622039</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1122,7 +1122,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>21864.3161792</v>
+        <v>2027.446640569997</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1131,7 +1131,7 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>2027.446640569997</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1139,7 +1139,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>1.67704221999999</v>
+        <v>1081.26268381</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1081.26268381</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1156,7 +1156,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>4000.98649741</v>
+        <v>3937.684245129999</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1165,7 +1165,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>3937.684245129999</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1173,13 +1173,13 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>0.709887740000002</v>
+        <v>60.52008236</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1190,7 +1190,7 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>5.43975284</v>
+        <v>20.02671061</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1199,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>20.02671061</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1207,7 +1207,7 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>492.6416848799999</v>
+        <v>634.7054047399988</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1216,7 +1216,7 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>634.7054047399988</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1224,7 +1224,7 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>3507.03044283</v>
+        <v>0.26138826</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1233,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>0.26138826</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1241,7 +1241,7 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>1641.07355304</v>
+        <v>6.87069001</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1250,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>6.87069001</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1258,7 +1258,7 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>4905.49194222</v>
+        <v>756.4421111899999</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1267,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>756.4421111899999</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1275,7 +1275,7 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>981.4251657099986</v>
+        <v>259.008</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1284,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>259.008</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1292,7 +1292,7 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>1.88259526</v>
+        <v>757.688</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1301,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>757.688</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1309,7 +1309,7 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>4.46240989</v>
+        <v>1020.985</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1318,7 +1318,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1020.985</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1326,13 +1326,13 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>697.0416251500001</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>49.312</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>49.312</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1343,13 +1343,13 @@
         <v>30</v>
       </c>
       <c r="B27">
-        <v>6.874403710000001</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>51.872</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>51.872</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1360,7 +1360,7 @@
         <v>31</v>
       </c>
       <c r="B28">
-        <v>2.17033882999997</v>
+        <v>3.242</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1369,7 +1369,7 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>3.242</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1377,7 +1377,7 @@
         <v>32</v>
       </c>
       <c r="B29">
-        <v>16.76622039</v>
+        <v>54.432</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1386,7 +1386,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>54.432</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1394,13 +1394,13 @@
         <v>33</v>
       </c>
       <c r="B30">
-        <v>283.614</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>91.854</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>91.854</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1411,7 +1411,7 @@
         <v>34</v>
       </c>
       <c r="B31">
-        <v>2760.418009269995</v>
+        <v>3.402</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1420,7 +1420,7 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>3.402</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1428,16 +1428,16 @@
         <v>35</v>
       </c>
       <c r="B32">
-        <v>4481.60575281</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <v>3000</v>
+        <v>2</v>
       </c>
       <c r="D32">
-        <v>2700</v>
+        <v>2</v>
       </c>
       <c r="E32">
-        <v>1481.60575281</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1445,7 +1445,7 @@
         <v>36</v>
       </c>
       <c r="B33">
-        <v>6642.509878519999</v>
+        <v>0.09183673000000001</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1454,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>0.09183673000000001</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1462,13 +1462,13 @@
         <v>37</v>
       </c>
       <c r="B34">
-        <v>127.66323376</v>
+        <v>0</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1479,7 +1479,7 @@
         <v>38</v>
       </c>
       <c r="B35">
-        <v>376.09794026</v>
+        <v>26.81442857</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1488,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>26.81442857</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1496,7 +1496,7 @@
         <v>39</v>
       </c>
       <c r="B36">
-        <v>350.20391349</v>
+        <v>0.05204082</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1505,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>0.05204082</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1513,7 +1513,7 @@
         <v>40</v>
       </c>
       <c r="B37">
-        <v>183.6565561300002</v>
+        <v>16</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1522,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1530,13 +1530,13 @@
         <v>41</v>
       </c>
       <c r="B38">
-        <v>0.26138826</v>
+        <v>0</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1547,7 +1547,7 @@
         <v>42</v>
       </c>
       <c r="B39">
-        <v>5.71420804999979</v>
+        <v>25.2</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1556,7 +1556,7 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1564,13 +1564,13 @@
         <v>43</v>
       </c>
       <c r="B40">
-        <v>9.882429450000011</v>
+        <v>0</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>25.2</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>25.2</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -1581,7 +1581,7 @@
         <v>44</v>
       </c>
       <c r="B41">
-        <v>133.14315139</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1590,7 +1590,7 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>8.800000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1598,13 +1598,13 @@
         <v>45</v>
       </c>
       <c r="B42">
-        <v>1209.45112659</v>
+        <v>0</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -1615,7 +1615,7 @@
         <v>46</v>
       </c>
       <c r="B43">
-        <v>9.215999999999999</v>
+        <v>0.016</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1624,7 +1624,7 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1632,7 +1632,7 @@
         <v>47</v>
       </c>
       <c r="B44">
-        <v>1602.84</v>
+        <v>226</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1641,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>226</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1649,13 +1649,13 @@
         <v>48</v>
       </c>
       <c r="B45">
-        <v>1065.177</v>
+        <v>0</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1666,13 +1666,13 @@
         <v>49</v>
       </c>
       <c r="B46">
-        <v>399.636</v>
+        <v>10</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -1683,7 +1683,7 @@
         <v>50</v>
       </c>
       <c r="B47">
-        <v>51.872</v>
+        <v>0.0638517</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1692,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>0.0638517</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1700,7 +1700,7 @@
         <v>51</v>
       </c>
       <c r="B48">
-        <v>3.242</v>
+        <v>82.9389660099999</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1709,7 +1709,7 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>82.9389660099999</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1717,13 +1717,13 @@
         <v>52</v>
       </c>
       <c r="B49">
-        <v>13.608</v>
+        <v>54.28240062</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -1734,7 +1734,7 @@
         <v>53</v>
       </c>
       <c r="B50">
-        <v>54.432</v>
+        <v>416.08485585</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1743,7 +1743,7 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>416.08485585</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1751,7 +1751,7 @@
         <v>54</v>
       </c>
       <c r="B51">
-        <v>88.452</v>
+        <v>1782.8109423</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1760,7 +1760,7 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>1782.8109423</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1768,13 +1768,13 @@
         <v>55</v>
       </c>
       <c r="B52">
-        <v>3.402</v>
+        <v>430.8393408899988</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -1785,7 +1785,7 @@
         <v>56</v>
       </c>
       <c r="B53">
-        <v>0.2122449</v>
+        <v>2.94335736</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -1794,7 +1794,7 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>2.94335736</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1802,7 +1802,7 @@
         <v>57</v>
       </c>
       <c r="B54">
-        <v>0.47551021</v>
+        <v>1845.05699075</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -1811,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>1845.05699075</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1819,7 +1819,7 @@
         <v>58</v>
       </c>
       <c r="B55">
-        <v>0.09183673000000001</v>
+        <v>3555.490545809999</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -1828,7 +1828,7 @@
         <v>0</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>3555.490545809999</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1836,16 +1836,16 @@
         <v>59</v>
       </c>
       <c r="B56">
-        <v>0.2122449</v>
+        <v>186.7796086599999</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>56.77960865999989</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1853,7 +1853,7 @@
         <v>60</v>
       </c>
       <c r="B57">
-        <v>20.41442856999999</v>
+        <v>68.10011535</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1862,7 +1862,7 @@
         <v>0</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>68.10011535</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1870,7 +1870,7 @@
         <v>61</v>
       </c>
       <c r="B58">
-        <v>0.05204082</v>
+        <v>314.4481565099999</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1879,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>314.4481565099999</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1887,7 +1887,7 @@
         <v>62</v>
       </c>
       <c r="B59">
-        <v>16</v>
+        <v>883.62768793</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1896,7 +1896,7 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>883.62768793</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1904,16 +1904,16 @@
         <v>63</v>
       </c>
       <c r="B60">
-        <v>25.2</v>
+        <v>655.49330589</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>495.49330589</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1921,7 +1921,7 @@
         <v>64</v>
       </c>
       <c r="B61">
-        <v>8.800000000000001</v>
+        <v>391.93716994</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1930,7 +1930,7 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>391.93716994</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1938,16 +1938,16 @@
         <v>65</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>1890.72350777</v>
       </c>
       <c r="C62">
-        <v>9.6</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>8.640000000000001</v>
+        <v>0</v>
       </c>
       <c r="E62">
-        <v>-9.6</v>
+        <v>1890.72350777</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1955,13 +1955,13 @@
         <v>66</v>
       </c>
       <c r="B63">
-        <v>558</v>
+        <v>123.62512873</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>155.6</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>155.6</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -1972,7 +1972,7 @@
         <v>67</v>
       </c>
       <c r="B64">
-        <v>0.04222451</v>
+        <v>3.43357364</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1981,7 +1981,7 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>3.43357364</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1989,7 +1989,7 @@
         <v>68</v>
       </c>
       <c r="B65">
-        <v>294.26902061</v>
+        <v>4.992</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1998,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>4.992</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2006,7 +2006,7 @@
         <v>69</v>
       </c>
       <c r="B66">
-        <v>512.32245619</v>
+        <v>51.614</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -2015,7 +2015,7 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>51.614</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2023,13 +2023,13 @@
         <v>70</v>
       </c>
       <c r="B67">
-        <v>359.9673151399989</v>
+        <v>0</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -2040,13 +2040,13 @@
         <v>71</v>
       </c>
       <c r="B68">
-        <v>129.47314934</v>
+        <v>0</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -2057,13 +2057,13 @@
         <v>72</v>
       </c>
       <c r="B69">
-        <v>1850.60880743</v>
+        <v>0</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -2074,16 +2074,16 @@
         <v>73</v>
       </c>
       <c r="B70">
-        <v>7771.982495420001</v>
+        <v>0</v>
       </c>
       <c r="C70">
-        <v>1080</v>
+        <v>6</v>
       </c>
       <c r="D70">
-        <v>972</v>
+        <v>6</v>
       </c>
       <c r="E70">
-        <v>6691.982495420001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2091,16 +2091,16 @@
         <v>74</v>
       </c>
       <c r="B71">
-        <v>941.6731617199998</v>
+        <v>33</v>
       </c>
       <c r="C71">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="D71">
-        <v>86.40000000000001</v>
+        <v>135</v>
       </c>
       <c r="E71">
-        <v>845.6731617199998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2108,7 +2108,7 @@
         <v>75</v>
       </c>
       <c r="B72">
-        <v>2.94335736</v>
+        <v>624</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -2117,7 +2117,7 @@
         <v>0</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>624</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2125,16 +2125,16 @@
         <v>76</v>
       </c>
       <c r="B73">
-        <v>4765.2015046</v>
+        <v>6</v>
       </c>
       <c r="C73">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="D73">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="E73">
-        <v>4665.2015046</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2142,16 +2142,16 @@
         <v>77</v>
       </c>
       <c r="B74">
-        <v>3960.65016162</v>
+        <v>0</v>
       </c>
       <c r="C74">
-        <v>1080</v>
+        <v>459</v>
       </c>
       <c r="D74">
-        <v>972</v>
+        <v>459</v>
       </c>
       <c r="E74">
-        <v>2880.65016162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2159,13 +2159,13 @@
         <v>78</v>
       </c>
       <c r="B75">
-        <v>168.5571575799989</v>
+        <v>0</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -2176,13 +2176,13 @@
         <v>79</v>
       </c>
       <c r="B76">
-        <v>264.14585067</v>
+        <v>0</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -2193,16 +2193,16 @@
         <v>80</v>
       </c>
       <c r="B77">
-        <v>1309.9208826</v>
+        <v>0</v>
       </c>
       <c r="C77">
-        <v>1080</v>
+        <v>1</v>
       </c>
       <c r="D77">
-        <v>972</v>
+        <v>1</v>
       </c>
       <c r="E77">
-        <v>229.9208825999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2210,13 +2210,13 @@
         <v>81</v>
       </c>
       <c r="B78">
-        <v>1459.45538722</v>
+        <v>0</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -2227,16 +2227,16 @@
         <v>82</v>
       </c>
       <c r="B79">
-        <v>2076.35721215999</v>
+        <v>0</v>
       </c>
       <c r="C79">
-        <v>1080</v>
+        <v>1</v>
       </c>
       <c r="D79">
-        <v>972</v>
+        <v>1</v>
       </c>
       <c r="E79">
-        <v>996.3572121599896</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2244,13 +2244,13 @@
         <v>83</v>
       </c>
       <c r="B80">
-        <v>751.419155539999</v>
+        <v>0</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -2261,13 +2261,13 @@
         <v>84</v>
       </c>
       <c r="B81">
-        <v>43.53347064</v>
+        <v>0</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -2278,13 +2278,13 @@
         <v>85</v>
       </c>
       <c r="B82">
-        <v>1711.35259527</v>
+        <v>0</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -2295,13 +2295,13 @@
         <v>86</v>
       </c>
       <c r="B83">
-        <v>2892.79520088</v>
+        <v>0</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -2312,13 +2312,13 @@
         <v>87</v>
       </c>
       <c r="B84">
-        <v>123.62512873</v>
+        <v>0</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -2329,7 +2329,7 @@
         <v>88</v>
       </c>
       <c r="B85">
-        <v>3.43357364</v>
+        <v>624</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2338,7 +2338,7 @@
         <v>0</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>624</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2346,7 +2346,7 @@
         <v>89</v>
       </c>
       <c r="B86">
-        <v>4.992</v>
+        <v>33</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2355,7 +2355,7 @@
         <v>0</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2363,16 +2363,16 @@
         <v>90</v>
       </c>
       <c r="B87">
-        <v>341</v>
+        <v>40</v>
       </c>
       <c r="C87">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="D87">
-        <v>57.6</v>
+        <v>0</v>
       </c>
       <c r="E87">
-        <v>277</v>
+        <v>40</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2380,7 +2380,7 @@
         <v>91</v>
       </c>
       <c r="B88">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2389,7 +2389,7 @@
         <v>0</v>
       </c>
       <c r="E88">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2397,7 +2397,7 @@
         <v>92</v>
       </c>
       <c r="B89">
-        <v>372</v>
+        <v>128</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2406,7 +2406,7 @@
         <v>0</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>128</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2414,7 +2414,7 @@
         <v>93</v>
       </c>
       <c r="B90">
-        <v>624</v>
+        <v>0.192</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2423,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>0.192</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -2431,7 +2431,7 @@
         <v>94</v>
       </c>
       <c r="B91">
-        <v>392</v>
+        <v>350</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2440,7 +2440,7 @@
         <v>0</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>350</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2448,7 +2448,7 @@
         <v>95</v>
       </c>
       <c r="B92">
-        <v>513</v>
+        <v>1</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -2457,7 +2457,7 @@
         <v>0</v>
       </c>
       <c r="E92">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2465,7 +2465,7 @@
         <v>96</v>
       </c>
       <c r="B93">
-        <v>191</v>
+        <v>2</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -2474,7 +2474,7 @@
         <v>0</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2482,7 +2482,7 @@
         <v>97</v>
       </c>
       <c r="B94">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -2491,7 +2491,7 @@
         <v>0</v>
       </c>
       <c r="E94">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2499,7 +2499,7 @@
         <v>98</v>
       </c>
       <c r="B95">
-        <v>0.024</v>
+        <v>5</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -2508,7 +2508,7 @@
         <v>0</v>
       </c>
       <c r="E95">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2516,16 +2516,16 @@
         <v>99</v>
       </c>
       <c r="B96">
-        <v>48</v>
+        <v>7.6</v>
       </c>
       <c r="C96">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D96">
-        <v>7.2</v>
+        <v>0</v>
       </c>
       <c r="E96">
-        <v>40</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2533,16 +2533,16 @@
         <v>100</v>
       </c>
       <c r="B97">
-        <v>973</v>
+        <v>10</v>
       </c>
       <c r="C97">
-        <v>594</v>
+        <v>0</v>
       </c>
       <c r="D97">
-        <v>534.6</v>
+        <v>0</v>
       </c>
       <c r="E97">
-        <v>379</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2550,10 +2550,10 @@
         <v>101</v>
       </c>
       <c r="B98">
-        <v>564</v>
+        <v>0</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>1.76</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -2567,16 +2567,16 @@
         <v>102</v>
       </c>
       <c r="B99">
-        <v>1104</v>
+        <v>1.08</v>
       </c>
       <c r="C99">
-        <v>1104</v>
+        <v>0</v>
       </c>
       <c r="D99">
-        <v>993.6</v>
+        <v>0</v>
       </c>
       <c r="E99">
-        <v>0</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2584,7 +2584,7 @@
         <v>103</v>
       </c>
       <c r="B100">
-        <v>624</v>
+        <v>87.13499999999998</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -2593,7 +2593,7 @@
         <v>0</v>
       </c>
       <c r="E100">
-        <v>0</v>
+        <v>87.13499999999998</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2601,7 +2601,7 @@
         <v>104</v>
       </c>
       <c r="B101">
-        <v>6</v>
+        <v>26.2079999999999</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -2610,7 +2610,7 @@
         <v>0</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>26.2079999999999</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2618,16 +2618,16 @@
         <v>105</v>
       </c>
       <c r="B102">
-        <v>67</v>
+        <v>194.579999999999</v>
       </c>
       <c r="C102">
-        <v>214</v>
+        <v>0</v>
       </c>
       <c r="D102">
-        <v>192.6</v>
+        <v>0</v>
       </c>
       <c r="E102">
-        <v>-147</v>
+        <v>194.579999999999</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2635,7 +2635,7 @@
         <v>106</v>
       </c>
       <c r="B103">
-        <v>120</v>
+        <v>165.451999999999</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -2644,7 +2644,7 @@
         <v>0</v>
       </c>
       <c r="E103">
-        <v>0</v>
+        <v>165.451999999999</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2652,7 +2652,7 @@
         <v>107</v>
       </c>
       <c r="B104">
-        <v>26</v>
+        <v>227.772</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -2661,7 +2661,7 @@
         <v>0</v>
       </c>
       <c r="E104">
-        <v>0</v>
+        <v>227.772</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2669,16 +2669,16 @@
         <v>108</v>
       </c>
       <c r="B105">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C105">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="D105">
-        <v>47.7</v>
+        <v>0</v>
       </c>
       <c r="E105">
-        <v>-53</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2686,7 +2686,7 @@
         <v>109</v>
       </c>
       <c r="B106">
-        <v>339</v>
+        <v>1</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -2695,7 +2695,7 @@
         <v>0</v>
       </c>
       <c r="E106">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2703,16 +2703,16 @@
         <v>110</v>
       </c>
       <c r="B107">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C107">
-        <v>4</v>
+        <v>459</v>
       </c>
       <c r="D107">
-        <v>3.6</v>
+        <v>459</v>
       </c>
       <c r="E107">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2720,16 +2720,16 @@
         <v>111</v>
       </c>
       <c r="B108">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="C108">
-        <v>16</v>
+        <v>244</v>
       </c>
       <c r="D108">
-        <v>14.4</v>
+        <v>244</v>
       </c>
       <c r="E108">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2740,10 +2740,10 @@
         <v>6</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D109">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E109">
         <v>0</v>
@@ -2754,13 +2754,13 @@
         <v>113</v>
       </c>
       <c r="B110">
-        <v>437</v>
+        <v>448</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>490</v>
       </c>
       <c r="D110">
-        <v>0</v>
+        <v>490</v>
       </c>
       <c r="E110">
         <v>0</v>
@@ -2771,13 +2771,13 @@
         <v>114</v>
       </c>
       <c r="B111">
-        <v>549</v>
+        <v>141</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>411</v>
       </c>
       <c r="D111">
-        <v>0</v>
+        <v>411</v>
       </c>
       <c r="E111">
         <v>0</v>
@@ -2788,7 +2788,7 @@
         <v>115</v>
       </c>
       <c r="B112">
-        <v>933</v>
+        <v>0.2</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2797,7 +2797,7 @@
         <v>0</v>
       </c>
       <c r="E112">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2805,7 +2805,7 @@
         <v>116</v>
       </c>
       <c r="B113">
-        <v>5</v>
+        <v>0.2</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2814,7 +2814,7 @@
         <v>0</v>
       </c>
       <c r="E113">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2822,7 +2822,7 @@
         <v>117</v>
       </c>
       <c r="B114">
-        <v>235</v>
+        <v>1488</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -2831,7 +2831,7 @@
         <v>0</v>
       </c>
       <c r="E114">
-        <v>0</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -2839,7 +2839,7 @@
         <v>118</v>
       </c>
       <c r="B115">
-        <v>192</v>
+        <v>41</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -2848,7 +2848,7 @@
         <v>0</v>
       </c>
       <c r="E115">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -2856,13 +2856,13 @@
         <v>119</v>
       </c>
       <c r="B116">
-        <v>1488</v>
+        <v>0</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E116">
         <v>0</v>
@@ -2873,13 +2873,13 @@
         <v>120</v>
       </c>
       <c r="B117">
-        <v>575</v>
+        <v>0</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E117">
         <v>0</v>
@@ -2890,16 +2890,16 @@
         <v>121</v>
       </c>
       <c r="B118">
-        <v>1025</v>
+        <v>575</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E118">
-        <v>0</v>
+        <v>574</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -2907,13 +2907,13 @@
         <v>122</v>
       </c>
       <c r="B119">
-        <v>242</v>
+        <v>0</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>1838</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>1838</v>
       </c>
       <c r="E119">
         <v>0</v>
@@ -2924,16 +2924,16 @@
         <v>123</v>
       </c>
       <c r="B120">
-        <v>509</v>
+        <v>413</v>
       </c>
       <c r="C120">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D120">
-        <v>14.4</v>
+        <v>1</v>
       </c>
       <c r="E120">
-        <v>493</v>
+        <v>412</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -2941,16 +2941,16 @@
         <v>124</v>
       </c>
       <c r="B121">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="C121">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D121">
-        <v>3.6</v>
+        <v>0</v>
       </c>
       <c r="E121">
-        <v>-1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -2958,7 +2958,7 @@
         <v>125</v>
       </c>
       <c r="B122">
-        <v>36</v>
+        <v>1.1</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -2967,7 +2967,7 @@
         <v>0</v>
       </c>
       <c r="E122">
-        <v>0</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -2975,13 +2975,13 @@
         <v>126</v>
       </c>
       <c r="B123">
-        <v>488</v>
+        <v>0</v>
       </c>
       <c r="C123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E123">
         <v>0</v>
@@ -2992,13 +2992,13 @@
         <v>127</v>
       </c>
       <c r="B124">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>307</v>
       </c>
       <c r="D124">
-        <v>0</v>
+        <v>307</v>
       </c>
       <c r="E124">
         <v>0</v>
@@ -3009,13 +3009,13 @@
         <v>128</v>
       </c>
       <c r="B125">
-        <v>2748</v>
+        <v>0</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E125">
         <v>0</v>
@@ -3026,13 +3026,13 @@
         <v>129</v>
       </c>
       <c r="B126">
-        <v>467</v>
+        <v>0</v>
       </c>
       <c r="C126">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="D126">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="E126">
         <v>0</v>
@@ -3043,7 +3043,7 @@
         <v>130</v>
       </c>
       <c r="B127">
-        <v>3.92</v>
+        <v>1380</v>
       </c>
       <c r="C127">
         <v>0</v>
@@ -3052,7 +3052,7 @@
         <v>0</v>
       </c>
       <c r="E127">
-        <v>0</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -3060,16 +3060,16 @@
         <v>131</v>
       </c>
       <c r="B128">
-        <v>48.96</v>
+        <v>467</v>
       </c>
       <c r="C128">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E128">
-        <v>0</v>
+        <v>466</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -3077,13 +3077,13 @@
         <v>132</v>
       </c>
       <c r="B129">
-        <v>1000.959999999999</v>
+        <v>0</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E129">
         <v>0</v>
@@ -3094,16 +3094,16 @@
         <v>133</v>
       </c>
       <c r="B130">
-        <v>772.4799999999999</v>
+        <v>0</v>
       </c>
       <c r="C130">
-        <v>408</v>
+        <v>1</v>
       </c>
       <c r="D130">
-        <v>367.2</v>
+        <v>1</v>
       </c>
       <c r="E130">
-        <v>364.4799999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -3111,7 +3111,7 @@
         <v>134</v>
       </c>
       <c r="B131">
-        <v>32.4</v>
+        <v>48</v>
       </c>
       <c r="C131">
         <v>0</v>
@@ -3120,7 +3120,7 @@
         <v>0</v>
       </c>
       <c r="E131">
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -3128,7 +3128,7 @@
         <v>135</v>
       </c>
       <c r="B132">
-        <v>2.22044604925031e-15</v>
+        <v>24</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -3137,7 +3137,7 @@
         <v>0</v>
       </c>
       <c r="E132">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -3145,7 +3145,7 @@
         <v>136</v>
       </c>
       <c r="B133">
-        <v>244.967606589999</v>
+        <v>3.92</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -3154,7 +3154,7 @@
         <v>0</v>
       </c>
       <c r="E133">
-        <v>0</v>
+        <v>3.92</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -3162,10 +3162,10 @@
         <v>137</v>
       </c>
       <c r="B134">
-        <v>20.39443872999999</v>
+        <v>12.64</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>272</v>
       </c>
       <c r="D134">
         <v>0</v>
@@ -3179,7 +3179,7 @@
         <v>138</v>
       </c>
       <c r="B135">
-        <v>592.7022451599991</v>
+        <v>569.4399999999999</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -3188,7 +3188,7 @@
         <v>0</v>
       </c>
       <c r="E135">
-        <v>0</v>
+        <v>569.4399999999999</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -3196,13 +3196,13 @@
         <v>139</v>
       </c>
       <c r="B136">
-        <v>39.95868998999999</v>
+        <v>0</v>
       </c>
       <c r="C136">
-        <v>0</v>
+        <v>71.68000000000001</v>
       </c>
       <c r="D136">
-        <v>0</v>
+        <v>71.68000000000001</v>
       </c>
       <c r="E136">
         <v>0</v>
@@ -3213,7 +3213,7 @@
         <v>140</v>
       </c>
       <c r="B137">
-        <v>14.90965084999999</v>
+        <v>26.88</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -3222,7 +3222,7 @@
         <v>0</v>
       </c>
       <c r="E137">
-        <v>0</v>
+        <v>26.88</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -3230,7 +3230,7 @@
         <v>141</v>
       </c>
       <c r="B138">
-        <v>4.03707518</v>
+        <v>282.2781328600001</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -3239,7 +3239,7 @@
         <v>0</v>
       </c>
       <c r="E138">
-        <v>0</v>
+        <v>282.2781328600001</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -3247,13 +3247,13 @@
         <v>142</v>
       </c>
       <c r="B139">
-        <v>168.03379502</v>
+        <v>0.9001029899999999</v>
       </c>
       <c r="C139">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="D139">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E139">
         <v>0</v>
@@ -3264,13 +3264,13 @@
         <v>143</v>
       </c>
       <c r="B140">
-        <v>1116.938433389999</v>
+        <v>0</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="D140">
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="E140">
         <v>0</v>
@@ -3281,16 +3281,16 @@
         <v>144</v>
       </c>
       <c r="B141">
-        <v>57.80066315000001</v>
+        <v>4.03707518</v>
       </c>
       <c r="C141">
-        <v>10.5</v>
+        <v>0</v>
       </c>
       <c r="D141">
-        <v>9.449999999999999</v>
+        <v>0</v>
       </c>
       <c r="E141">
-        <v>47.30066315000001</v>
+        <v>4.03707518</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -3298,7 +3298,7 @@
         <v>145</v>
       </c>
       <c r="B142">
-        <v>0.42430484</v>
+        <v>123.54798453</v>
       </c>
       <c r="C142">
         <v>0</v>
@@ -3307,7 +3307,7 @@
         <v>0</v>
       </c>
       <c r="E142">
-        <v>0</v>
+        <v>123.54798453</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -3315,13 +3315,13 @@
         <v>146</v>
       </c>
       <c r="B143">
-        <v>0.10504634</v>
+        <v>30.79690826</v>
       </c>
       <c r="C143">
-        <v>0</v>
+        <v>425</v>
       </c>
       <c r="D143">
-        <v>0</v>
+        <v>425</v>
       </c>
       <c r="E143">
         <v>0</v>
@@ -3332,7 +3332,7 @@
         <v>147</v>
       </c>
       <c r="B144">
-        <v>418.4624098899999</v>
+        <v>0.42430484</v>
       </c>
       <c r="C144">
         <v>0</v>
@@ -3341,7 +3341,7 @@
         <v>0</v>
       </c>
       <c r="E144">
-        <v>0</v>
+        <v>0.42430484</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -3349,7 +3349,7 @@
         <v>148</v>
       </c>
       <c r="B145">
-        <v>13.141018580001</v>
+        <v>0.10504634</v>
       </c>
       <c r="C145">
         <v>0</v>
@@ -3358,7 +3358,7 @@
         <v>0</v>
       </c>
       <c r="E145">
-        <v>0</v>
+        <v>0.10504634</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -3366,7 +3366,7 @@
         <v>149</v>
       </c>
       <c r="B146">
-        <v>567.8916034899989</v>
+        <v>427.28565085</v>
       </c>
       <c r="C146">
         <v>0</v>
@@ -3375,7 +3375,7 @@
         <v>0</v>
       </c>
       <c r="E146">
-        <v>0</v>
+        <v>427.28565085</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -3383,7 +3383,7 @@
         <v>150</v>
       </c>
       <c r="B147">
-        <v>1.19876415</v>
+        <v>21.6262934699997</v>
       </c>
       <c r="C147">
         <v>0</v>
@@ -3392,7 +3392,7 @@
         <v>0</v>
       </c>
       <c r="E147">
-        <v>0</v>
+        <v>21.6262934699997</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -3400,7 +3400,7 @@
         <v>151</v>
       </c>
       <c r="B148">
-        <v>0.1338826</v>
+        <v>3.08341916</v>
       </c>
       <c r="C148">
         <v>0</v>
@@ -3409,7 +3409,7 @@
         <v>0</v>
       </c>
       <c r="E148">
-        <v>0</v>
+        <v>3.08341916</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -3417,7 +3417,7 @@
         <v>152</v>
       </c>
       <c r="B149">
-        <v>337.43350152</v>
+        <v>0.1338826</v>
       </c>
       <c r="C149">
         <v>0</v>
@@ -3426,7 +3426,7 @@
         <v>0</v>
       </c>
       <c r="E149">
-        <v>0</v>
+        <v>0.1338826</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -3434,7 +3434,7 @@
         <v>153</v>
       </c>
       <c r="B150">
-        <v>12.13182286</v>
+        <v>245.88204427</v>
       </c>
       <c r="C150">
         <v>0</v>
@@ -3443,7 +3443,7 @@
         <v>0</v>
       </c>
       <c r="E150">
-        <v>0</v>
+        <v>245.88204427</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -3451,13 +3451,13 @@
         <v>154</v>
       </c>
       <c r="B151">
-        <v>0.75798146</v>
+        <v>12.13182286</v>
       </c>
       <c r="C151">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="D151">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="E151">
         <v>0</v>
@@ -3468,16 +3468,16 @@
         <v>155</v>
       </c>
       <c r="B152">
-        <v>0</v>
+        <v>0.75798146</v>
       </c>
       <c r="C152">
-        <v>0.5760000000000001</v>
+        <v>0</v>
       </c>
       <c r="D152">
-        <v>0.5184</v>
+        <v>0</v>
       </c>
       <c r="E152">
-        <v>-0.5760000000000001</v>
+        <v>0.75798146</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -3485,7 +3485,7 @@
         <v>156</v>
       </c>
       <c r="B153">
-        <v>0.0995180299999999</v>
+        <v>1.8</v>
       </c>
       <c r="C153">
         <v>0</v>
@@ -3494,7 +3494,7 @@
         <v>0</v>
       </c>
       <c r="E153">
-        <v>0</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -3502,7 +3502,7 @@
         <v>157</v>
       </c>
       <c r="B154">
-        <v>28.71266735</v>
+        <v>1.62</v>
       </c>
       <c r="C154">
         <v>0</v>
@@ -3511,7 +3511,7 @@
         <v>0</v>
       </c>
       <c r="E154">
-        <v>0</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -3519,7 +3519,7 @@
         <v>158</v>
       </c>
       <c r="B155">
-        <v>162.996</v>
+        <v>0.88</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -3528,7 +3528,7 @@
         <v>0</v>
       </c>
       <c r="E155">
-        <v>0</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -3536,7 +3536,7 @@
         <v>159</v>
       </c>
       <c r="B156">
-        <v>1.8</v>
+        <v>1.52</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -3545,7 +3545,7 @@
         <v>0</v>
       </c>
       <c r="E156">
-        <v>0</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -3553,7 +3553,7 @@
         <v>160</v>
       </c>
       <c r="B157">
-        <v>1.62</v>
+        <v>61.28</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -3562,7 +3562,7 @@
         <v>0</v>
       </c>
       <c r="E157">
-        <v>0</v>
+        <v>61.28</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -3570,13 +3570,13 @@
         <v>161</v>
       </c>
       <c r="B158">
-        <v>0.88</v>
+        <v>0</v>
       </c>
       <c r="C158">
-        <v>0</v>
+        <v>61.28</v>
       </c>
       <c r="D158">
-        <v>0</v>
+        <v>61.28</v>
       </c>
       <c r="E158">
         <v>0</v>
@@ -3587,13 +3587,13 @@
         <v>162</v>
       </c>
       <c r="B159">
-        <v>1.52</v>
+        <v>0</v>
       </c>
       <c r="C159">
-        <v>0</v>
+        <v>780.415</v>
       </c>
       <c r="D159">
-        <v>0</v>
+        <v>780.415</v>
       </c>
       <c r="E159">
         <v>0</v>
@@ -3604,16 +3604,16 @@
         <v>163</v>
       </c>
       <c r="B160">
-        <v>61.28</v>
+        <v>8880.799999999999</v>
       </c>
       <c r="C160">
-        <v>0</v>
+        <v>1567.2</v>
       </c>
       <c r="D160">
-        <v>0</v>
+        <v>1567.2</v>
       </c>
       <c r="E160">
-        <v>0</v>
+        <v>7313.599999999999</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -3621,13 +3621,13 @@
         <v>164</v>
       </c>
       <c r="B161">
-        <v>10448</v>
+        <v>192.199999999999</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>281.48</v>
       </c>
       <c r="D161">
-        <v>0</v>
+        <v>281.48</v>
       </c>
       <c r="E161">
         <v>0</v>
@@ -3638,13 +3638,13 @@
         <v>165</v>
       </c>
       <c r="B162">
-        <v>4.96</v>
+        <v>0</v>
       </c>
       <c r="C162">
-        <v>0</v>
+        <v>1075</v>
       </c>
       <c r="D162">
-        <v>0</v>
+        <v>430</v>
       </c>
       <c r="E162">
         <v>0</v>
@@ -3655,7 +3655,7 @@
         <v>166</v>
       </c>
       <c r="B163">
-        <v>169.88</v>
+        <v>1.31</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -3664,7 +3664,7 @@
         <v>0</v>
       </c>
       <c r="E163">
-        <v>0</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -3672,7 +3672,7 @@
         <v>167</v>
       </c>
       <c r="B164">
-        <v>48.16</v>
+        <v>146.56</v>
       </c>
       <c r="C164">
         <v>0</v>
@@ -3681,7 +3681,7 @@
         <v>0</v>
       </c>
       <c r="E164">
-        <v>0</v>
+        <v>146.56</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -3689,10 +3689,10 @@
         <v>168</v>
       </c>
       <c r="B165">
-        <v>6.256</v>
+        <v>0</v>
       </c>
       <c r="C165">
-        <v>0</v>
+        <v>38.4</v>
       </c>
       <c r="D165">
         <v>0</v>
@@ -3706,16 +3706,16 @@
         <v>169</v>
       </c>
       <c r="B166">
-        <v>1.31</v>
+        <v>1220</v>
       </c>
       <c r="C166">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="D166">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="E166">
-        <v>0</v>
+        <v>620</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -3723,7 +3723,7 @@
         <v>170</v>
       </c>
       <c r="B167">
-        <v>146.56</v>
+        <v>2.4</v>
       </c>
       <c r="C167">
         <v>0</v>
@@ -3732,7 +3732,7 @@
         <v>0</v>
       </c>
       <c r="E167">
-        <v>0</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -3740,16 +3740,16 @@
         <v>171</v>
       </c>
       <c r="B168">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="C168">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D168">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="E168">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -3757,16 +3757,16 @@
         <v>172</v>
       </c>
       <c r="B169">
-        <v>1119</v>
+        <v>11</v>
       </c>
       <c r="C169">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D169">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E169">
-        <v>1019</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>